<commit_message>
Ya estan las graficas
</commit_message>
<xml_diff>
--- a/Gráfica.xlsx
+++ b/Gráfica.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ed. Chamo\Desktop\Trabajos GitHub\HDT3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejo\Documents\4to Semestre\Algoritmos\HDT3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8148"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -149,7 +149,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-GT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -657,6 +657,328 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Merge Sort con ordenados</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4.78</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.82</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>46.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>61.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Insertion Sort con ordenados</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>18.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>78.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38.299999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Buble Sort con ordenados</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>33.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>95.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -665,11 +987,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="378702672"/>
-        <c:axId val="378696144"/>
+        <c:axId val="270455152"/>
+        <c:axId val="270519768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="378702672"/>
+        <c:axId val="270455152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -732,7 +1054,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-GT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -770,15 +1092,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="378696144"/>
+        <c:crossAx val="270519768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="378696144"/>
+        <c:axId val="270519768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +1177,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-GT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -893,10 +1215,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-GT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="378702672"/>
+        <c:crossAx val="270455152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -936,7 +1258,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-GT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -966,7 +1288,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-GT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1569,7 +1891,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1834,23 +2156,23 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B3" sqref="B3:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1879,7 +2201,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>200</v>
       </c>
@@ -1892,14 +2214,23 @@
       <c r="D2">
         <v>14.7</v>
       </c>
+      <c r="E2">
+        <v>4.78</v>
+      </c>
       <c r="F2">
         <v>13.6</v>
       </c>
+      <c r="G2">
+        <v>18.2</v>
+      </c>
       <c r="H2">
         <v>20.7</v>
       </c>
+      <c r="I2">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>400</v>
       </c>
@@ -1912,14 +2243,23 @@
       <c r="D3">
         <v>85.7</v>
       </c>
+      <c r="E3">
+        <v>4.82</v>
+      </c>
       <c r="F3">
         <v>35</v>
       </c>
+      <c r="G3">
+        <v>31.2</v>
+      </c>
       <c r="H3">
         <v>20.5</v>
       </c>
+      <c r="I3">
+        <v>11.8</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>600</v>
       </c>
@@ -1932,14 +2272,23 @@
       <c r="D4">
         <v>38.9</v>
       </c>
+      <c r="E4">
+        <v>17</v>
+      </c>
       <c r="F4">
         <v>63.9</v>
       </c>
+      <c r="G4">
+        <v>40</v>
+      </c>
       <c r="H4">
         <v>41</v>
       </c>
+      <c r="I4">
+        <v>18.899999999999999</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>800</v>
       </c>
@@ -1952,14 +2301,23 @@
       <c r="D5">
         <v>61.9</v>
       </c>
+      <c r="E5">
+        <v>45.4</v>
+      </c>
       <c r="F5">
         <v>59.7</v>
       </c>
+      <c r="G5">
+        <v>56.7</v>
+      </c>
       <c r="H5">
         <v>42.5</v>
       </c>
+      <c r="I5">
+        <v>30.1</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1000</v>
       </c>
@@ -1972,14 +2330,23 @@
       <c r="D6">
         <v>49.6</v>
       </c>
+      <c r="E6">
+        <v>57.2</v>
+      </c>
       <c r="F6">
         <v>63.5</v>
       </c>
+      <c r="G6">
+        <v>72</v>
+      </c>
       <c r="H6">
         <v>39.4</v>
       </c>
+      <c r="I6">
+        <v>33.799999999999997</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1200</v>
       </c>
@@ -1992,14 +2359,23 @@
       <c r="D7">
         <v>68.900000000000006</v>
       </c>
+      <c r="E7">
+        <v>60.1</v>
+      </c>
       <c r="F7">
         <v>83.4</v>
       </c>
+      <c r="G7">
+        <v>78.400000000000006</v>
+      </c>
       <c r="H7">
         <v>64.8</v>
       </c>
+      <c r="I7">
+        <v>38</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1400</v>
       </c>
@@ -2012,14 +2388,23 @@
       <c r="D8">
         <v>68.5</v>
       </c>
+      <c r="E8">
+        <v>46.1</v>
+      </c>
       <c r="F8">
         <v>85.9</v>
       </c>
+      <c r="G8">
+        <v>126</v>
+      </c>
       <c r="H8">
         <v>52</v>
       </c>
+      <c r="I8">
+        <v>95.9</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1600</v>
       </c>
@@ -2032,14 +2417,23 @@
       <c r="D9">
         <v>109</v>
       </c>
+      <c r="E9">
+        <v>151</v>
+      </c>
       <c r="F9">
         <v>84.4</v>
       </c>
+      <c r="G9">
+        <v>71</v>
+      </c>
       <c r="H9">
         <v>62.3</v>
       </c>
+      <c r="I9">
+        <v>60.1</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1800</v>
       </c>
@@ -2052,14 +2446,23 @@
       <c r="D10">
         <v>113</v>
       </c>
+      <c r="E10">
+        <v>103</v>
+      </c>
       <c r="F10">
         <v>96.3</v>
       </c>
+      <c r="G10">
+        <v>307</v>
+      </c>
       <c r="H10">
         <v>65.599999999999994</v>
       </c>
+      <c r="I10">
+        <v>149</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2000</v>
       </c>
@@ -2072,14 +2475,23 @@
       <c r="D11">
         <v>193</v>
       </c>
+      <c r="E11">
+        <v>61.8</v>
+      </c>
       <c r="F11">
         <v>118</v>
       </c>
+      <c r="G11">
+        <v>38.299999999999997</v>
+      </c>
       <c r="H11">
         <v>73</v>
       </c>
+      <c r="I11">
+        <v>44.6</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H12" t="s">
         <v>9</v>
       </c>

</xml_diff>